<commit_message>
v1.1.0 Implement createBloombergExcelFile() and createThomsonExcelFile()
</commit_message>
<xml_diff>
--- a/samples/Thomson Reuters fund pricing template.xlsx
+++ b/samples/Thomson Reuters fund pricing template.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chinalifefranklinamc.sharepoint.com/sites/IT618/Shared Documents/General/20201223 Setup Bloomberg page for short term bond fund/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\gitlab\nav_automation\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_F25DC773A252ABDACC104800999E75105ADE58EF" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C612A0EC-EDDB-4A37-AE28-4719F648291D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E491EB-788E-4447-A240-B6C7BCF783E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="2220" windowWidth="17970" windowHeight="12135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ISIN Code</t>
   </si>
@@ -46,21 +46,6 @@
   </si>
   <si>
     <t>Shares Outstanding</t>
-  </si>
-  <si>
-    <t>HK0000664455</t>
-  </si>
-  <si>
-    <t>China Life Franklin Global-Short Term Bond B USD</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>China Life Franklin Global-Short Term Bond I USD</t>
-  </si>
-  <si>
-    <t>HK0000664489</t>
   </si>
 </sst>
 </file>
@@ -394,19 +379,19 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="45.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,51 +414,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>9.9896999999999991</v>
-      </c>
-      <c r="E2" s="1">
-        <v>248941791.98000002</v>
-      </c>
-      <c r="F2" s="1">
-        <v>3995918.24</v>
-      </c>
-      <c r="G2" s="1">
-        <v>400000</v>
-      </c>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>9.9887999999999995</v>
-      </c>
-      <c r="E3" s="1">
-        <v>248941791.98000002</v>
-      </c>
-      <c r="F3" s="1">
-        <v>244945873.74000001</v>
-      </c>
-      <c r="G3" s="1">
-        <v>24521823.787900001</v>
-      </c>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -481,6 +430,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3ABBA213F535143A2153FAFFCD4B404" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="00705d5726f6d16a2d41866951f40978">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56ce6572-a240-4cd6-8225-c99230995deb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="da66d2f5d03ddcf0575955673b1bb8c9" ns2:_="">
     <xsd:import namespace="56ce6572-a240-4cd6-8225-c99230995deb"/>
@@ -658,15 +616,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -674,13 +623,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{766F98BE-D463-464A-B718-79E3E404654A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD15CF1A-74A2-4849-9293-C8472767B575}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD15CF1A-74A2-4849-9293-C8472767B575}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{766F98BE-D463-464A-B718-79E3E404654A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="56ce6572-a240-4cd6-8225-c99230995deb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{250A36E6-C7E3-45DC-AF9D-860D94DF6B94}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{250A36E6-C7E3-45DC-AF9D-860D94DF6B94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>